<commit_message>
updated r1 to w1
</commit_message>
<xml_diff>
--- a/data_dictionary_vFINAL.xlsx
+++ b/data_dictionary_vFINAL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Puneet\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Folder\projects\canbrs-therapeutics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B579FC4-4F43-4BB2-B730-9F5D5EF40217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7139A0A-1FA7-49F7-B602-32AE19C4749B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,12 +85,6 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>r1, b2, as3, ain4, r0</t>
-  </si>
-  <si>
-    <t>r1=White, b2=Black, as3=Asian/PI, ain4=Native American, r0=Unknown</t>
-  </si>
-  <si>
     <t>v4</t>
   </si>
   <si>
@@ -254,6 +248,12 @@
   </si>
   <si>
     <t>Positive, Negative, Unknown</t>
+  </si>
+  <si>
+    <t>w1=White, b2=Black, as3=Asian/PI, ain4=Native American, r0=Unknown</t>
+  </si>
+  <si>
+    <t>w1, b2, as3, ain4, r0</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,21 +714,21 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -737,21 +737,21 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -760,61 +760,61 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -823,21 +823,21 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -846,21 +846,21 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -869,21 +869,21 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -892,21 +892,21 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -915,21 +915,21 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -938,21 +938,21 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
@@ -961,21 +961,21 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
@@ -984,10 +984,10 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>